<commit_message>
Fixing HSQLDB UUID type
</commit_message>
<xml_diff>
--- a/judo-tatami-asm2rdbms/model/RDBMS Data Types Hsqldb.xlsx
+++ b/judo-tatami-asm2rdbms/model/RDBMS Data Types Hsqldb.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Project/judo-generator/hu.blackbelt.judo.generator.transformer.runtime.rdbms/model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Project/judo-tatami/judo-tatami-asm2rdbms/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="21160"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21160"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -108,13 +116,13 @@
     <t>JUUID</t>
   </si>
   <si>
-    <t>BINARY</t>
+    <t>UUID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -491,12 +499,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -668,9 +678,7 @@
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="3">
-        <v>16</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>

</xml_diff>